<commit_message>
modified table for last time
</commit_message>
<xml_diff>
--- a/results/table.xlsx
+++ b/results/table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92e7e42702d5a5cc/Documents/UIUC/Courses/2017_Spring/IE_413/Project/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MATLAB\ge413\project\GE413_Project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13940" windowHeight="9300"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="13944" windowHeight="9300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>k</t>
   </si>
@@ -40,6 +40,9 @@
   <si>
     <t>Cost</t>
   </si>
+  <si>
+    <t>started 11:00</t>
+  </si>
 </sst>
 </file>
 
@@ -54,12 +57,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,8 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -91,6 +102,1078 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GA1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>58.890799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.684600000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68.8596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74.6828</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79.223600000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84.755600000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GA2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="2">
+                  <c:v>72.415944540727907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.693240901213173</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>87.521663778162917</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>93.081455805892546</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="521486784"/>
+        <c:axId val="521491096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="521486784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521491096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="521491096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521486784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,15 +1439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:I15"/>
+  <dimension ref="C5:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -387,7 +1470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>100</v>
       </c>
@@ -395,7 +1478,7 @@
         <v>58.890799999999999</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>130</v>
       </c>
@@ -403,7 +1486,7 @@
         <v>65.684600000000003</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>150</v>
       </c>
@@ -418,12 +1501,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>180</v>
       </c>
@@ -431,7 +1514,7 @@
         <v>74.6828</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>200</v>
       </c>
@@ -446,12 +1529,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>250</v>
       </c>
@@ -466,27 +1549,43 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15">
         <v>300</v>
       </c>
+      <c r="J15" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C15">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>325</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17">
         <v>350</v>
       </c>
-      <c r="G15">
+      <c r="G17">
         <f>13427/14425*100</f>
         <v>93.081455805892546</v>
       </c>
-      <c r="H15">
+      <c r="H17">
         <v>71</v>
       </c>
-      <c r="I15">
+      <c r="I17">
         <v>598</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>